<commit_message>
0.0.4: bugfix : getter/setter for NotNull properties have been defined as undefined.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectTsAnnotationSample2.xlsx
+++ b/meta/objects/BlancoValueObjectTsAnnotationSample2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816C865-8C7B-3C49-A70A-3C95B3326236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D7C33-C40C-7B45-982D-3536E50E392D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
   <si>
     <t>クラス名</t>
   </si>
@@ -290,18 +290,6 @@
     <phoneticPr fontId="7"/>
   </si>
   <si>
-    <t>JsonProperty\\NotNull</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>JsonAutoDetect</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>NotNull</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>Nullable</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -319,10 +307,6 @@
   </si>
   <si>
     <t>integer</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>JsonProperty</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
@@ -468,6 +452,13 @@
   </si>
   <si>
     <t>blanco\sample\valueobjectts\test</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>""</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1684,8 +1675,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1741,7 +1732,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1758,7 +1749,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
@@ -1775,7 +1766,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
@@ -1788,7 +1779,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="83" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B9" s="84"/>
       <c r="C9" s="10"/>
@@ -1796,7 +1787,7 @@
       <c r="E9" s="37"/>
       <c r="F9" s="11"/>
       <c r="G9" s="81" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="38"/>
@@ -1808,9 +1799,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
+      <c r="C10" s="10"/>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="11"/>
@@ -1863,7 +1852,9 @@
         <v>37</v>
       </c>
       <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
+      <c r="C13" s="68" t="s">
+        <v>74</v>
+      </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1875,14 +1866,12 @@
     </row>
     <row r="14" spans="1:13" s="33" customFormat="1">
       <c r="A14" s="66" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B14" s="67"/>
-      <c r="C14" s="68" t="s">
-        <v>45</v>
-      </c>
+      <c r="C14" s="68"/>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -1894,7 +1883,7 @@
     </row>
     <row r="15" spans="1:13" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B15" s="67"/>
       <c r="C15" s="68"/>
@@ -1909,12 +1898,12 @@
     </row>
     <row r="16" spans="1:13" s="33" customFormat="1">
       <c r="A16" s="95" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B16" s="96"/>
       <c r="C16" s="68"/>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
@@ -1926,12 +1915,10 @@
     </row>
     <row r="17" spans="1:15" s="33" customFormat="1">
       <c r="A17" s="66" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B17" s="67"/>
-      <c r="C17" s="68" t="s">
-        <v>45</v>
-      </c>
+      <c r="C17" s="68"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
@@ -1946,9 +1933,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="67"/>
-      <c r="C18" s="68" t="s">
-        <v>45</v>
-      </c>
+      <c r="C18" s="68"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -1977,14 +1962,14 @@
     </row>
     <row r="20" spans="1:15" s="33" customFormat="1">
       <c r="A20" s="95" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" s="96"/>
       <c r="C20" s="68" t="s">
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -2092,7 +2077,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -2114,7 +2099,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C28" s="46"/>
       <c r="D28" s="46"/>
@@ -2241,7 +2226,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42"/>
@@ -2307,7 +2292,7 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
@@ -2329,7 +2314,7 @@
         <v>32</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C40" s="46"/>
       <c r="D40" s="46"/>
@@ -2449,16 +2434,16 @@
         <v>6</v>
       </c>
       <c r="G46" s="90" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H46" s="90" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I46" s="93" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J46" s="93" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K46" s="88" t="s">
         <v>2</v>
@@ -2490,15 +2475,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="21"/>
-      <c r="E48" s="21" t="s">
-        <v>55</v>
-      </c>
+      <c r="E48" s="21"/>
       <c r="F48" s="21" t="s">
         <v>34</v>
       </c>
@@ -2524,16 +2507,16 @@
         <v>2</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D49" s="21"/>
-      <c r="E49" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="F49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21">
+        <v>0</v>
+      </c>
       <c r="G49" s="21"/>
       <c r="H49" s="78"/>
       <c r="I49" s="78"/>
@@ -2588,10 +2571,10 @@
         <v>25</v>
       </c>
       <c r="D51" s="21"/>
-      <c r="E51" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="G51" s="21"/>
       <c r="H51" s="78"/>
       <c r="I51" s="78"/>
@@ -2616,12 +2599,12 @@
         <v>20</v>
       </c>
       <c r="D52" s="21"/>
-      <c r="E52" s="21" t="s">
-        <v>49</v>
-      </c>
+      <c r="E52" s="21"/>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
-      <c r="H52" s="78"/>
+      <c r="H52" s="78" t="s">
+        <v>45</v>
+      </c>
       <c r="I52" s="78"/>
       <c r="J52" s="78"/>
       <c r="K52" s="21" t="s">
@@ -2767,10 +2750,10 @@
         <v>37</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F3" s="60" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H3" s="60" t="s">
         <v>38</v>
@@ -2785,7 +2768,7 @@
         <v>41</v>
       </c>
       <c r="P3" s="60" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2794,7 +2777,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="62" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H4" s="62"/>
       <c r="J4" s="62"/>

</xml_diff>

<commit_message>
0.0.7: remove @ from auto detect import path.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectTsAnnotationSample2.xlsx
+++ b/meta/objects/BlancoValueObjectTsAnnotationSample2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D7C33-C40C-7B45-982D-3536E50E392D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E91DC9A-9B03-804E-9061-5E9AF17F9F02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13760" yWindow="3520" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>クラス名</t>
   </si>
@@ -459,6 +459,10 @@
   </si>
   <si>
     <t>""</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>%</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1675,8 +1679,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1782,7 +1786,9 @@
         <v>67</v>
       </c>
       <c r="B9" s="84"/>
-      <c r="C9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="11"/>

</xml_diff>